<commit_message>
Add CSV and Excel Utils
</commit_message>
<xml_diff>
--- a/src/test/resources/users.xlsx
+++ b/src/test/resources/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>ivanka</t>
   </si>
@@ -47,6 +47,21 @@
   </si>
   <si>
     <t>shram</t>
+  </si>
+  <si>
+    <t>logincustomer</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Customer</t>
   </si>
 </sst>
 </file>
@@ -893,16 +908,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -918,8 +935,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -935,8 +958,14 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -951,6 +980,35 @@
       </c>
       <c r="E3" t="s">
         <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>